<commit_message>
cambios estudiante 1 word
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4.xlsx
+++ b/Docs/Tablas Lab 4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 04 - Ordenamientos Iterativos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Tareas\ESTRUC. DE DATOS Y ALGORITMOS\lab4\LabSorts-S04-G09\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E197636-5D23-49AC-AB0F-C814FF421F77}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76952C34-2116-484D-AB7E-15A5B00D7539}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" activeTab="5" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="6375" yWindow="2265" windowWidth="21600" windowHeight="11505" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,8 +663,8 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>609.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
@@ -831,35 +831,35 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>640.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>642.63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>644.63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>1287.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>1931.8899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>3219.1499999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>5151.0399999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>8370.1899999999987</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>13521.229999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,35 +998,35 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>56.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>66.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>76.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>86.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>106.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>116.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>126.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1252,7 +1252,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2494,8 +2494,8 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>609.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>20</c:v>
@@ -2911,7 +2911,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3233,35 +3233,35 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>640.63</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>642.63</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>644.63</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>1287.26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>1931.8899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21</c:v>
+                  <c:v>3219.1499999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34</c:v>
+                  <c:v>5151.0399999999991</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>8370.1899999999987</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>89</c:v>
+                  <c:v>13521.229999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3650,7 +3650,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3972,35 +3972,35 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>31.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>46.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29</c:v>
+                  <c:v>56.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39</c:v>
+                  <c:v>66.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49</c:v>
+                  <c:v>76.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>59</c:v>
+                  <c:v>86.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>69</c:v>
+                  <c:v>96.25</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>79</c:v>
+                  <c:v>106.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89</c:v>
+                  <c:v>116.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>99</c:v>
+                  <c:v>126.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4389,7 +4389,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7330,7 +7330,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{39C68510-AE01-4761-A7FB-5F1B76E923F7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="76" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7473,7 +7473,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8662051" cy="6288490"/>
+    <xdr:ext cx="8660230" cy="6291513"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -7827,19 +7827,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.1171875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.52734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.76171875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -7853,21 +7853,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
-      <c r="B2" s="4">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4">
-        <v>4</v>
+      <c r="B2">
+        <v>609.38</v>
+      </c>
+      <c r="C2">
+        <v>640.63</v>
+      </c>
+      <c r="D2">
+        <v>31.25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>2000</v>
       </c>
@@ -7879,10 +7879,10 @@
       </c>
       <c r="D3" s="4">
         <f>D2+15</f>
-        <v>19</v>
+        <v>46.25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>4000</v>
       </c>
@@ -7891,14 +7891,14 @@
       </c>
       <c r="C4" s="4">
         <f>C3+C2</f>
-        <v>3</v>
+        <v>642.63</v>
       </c>
       <c r="D4" s="4">
         <f t="shared" ref="D4:D11" si="0">D3+10</f>
-        <v>29</v>
+        <v>56.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>8000</v>
       </c>
@@ -7907,14 +7907,14 @@
       </c>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C11" si="1">C4+C3</f>
-        <v>5</v>
+        <v>644.63</v>
       </c>
       <c r="D5" s="4">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>66.25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>16000</v>
       </c>
@@ -7923,14 +7923,14 @@
       </c>
       <c r="C6" s="4">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>1287.26</v>
       </c>
       <c r="D6" s="4">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>76.25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
@@ -7939,14 +7939,14 @@
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>13</v>
+        <v>1931.8899999999999</v>
       </c>
       <c r="D7" s="4">
         <f t="shared" si="0"/>
-        <v>59</v>
+        <v>86.25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
@@ -7955,14 +7955,14 @@
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>21</v>
+        <v>3219.1499999999996</v>
       </c>
       <c r="D8" s="4">
         <f t="shared" si="0"/>
-        <v>69</v>
+        <v>96.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
@@ -7971,14 +7971,14 @@
       </c>
       <c r="C9" s="4">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>5151.0399999999991</v>
       </c>
       <c r="D9" s="4">
         <f t="shared" si="0"/>
-        <v>79</v>
+        <v>106.25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
@@ -7987,14 +7987,14 @@
       </c>
       <c r="C10" s="4">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>8370.1899999999987</v>
       </c>
       <c r="D10" s="4">
         <f t="shared" si="0"/>
-        <v>89</v>
+        <v>116.25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>512000</v>
       </c>
@@ -8003,14 +8003,14 @@
       </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>89</v>
+        <v>13521.229999999998</v>
       </c>
       <c r="D11" s="4">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>126.25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
@@ -8024,7 +8024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>1000</v>
       </c>
@@ -8038,7 +8038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>2000</v>
       </c>
@@ -8053,7 +8053,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>4000</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>8000</v>
       </c>
@@ -8085,7 +8085,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>16000</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>32000</v>
       </c>
@@ -8117,7 +8117,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>64000</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>128000</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>256000</v>
       </c>
@@ -8165,7 +8165,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>512000</v>
       </c>
@@ -8191,12 +8191,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8411,15 +8408,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8444,10 +8445,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>